<commit_message>
AVGpool Models + AvgPool WS
</commit_message>
<xml_diff>
--- a/Software/src/HardwareSpec/4x4_Mac_result_final.xlsx
+++ b/Software/src/HardwareSpec/4x4_Mac_result_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferga\Documents\CollegeWork\Thesis\Code\MNIST_QAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferga\Documents\CollegeWork\Thesis\Github\CNN-Hardware-Software-Codesign\Software\src\HardwareSpec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C545B18C-C281-493D-9A84-C22EB63CC35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297CB782-9B5D-4BFD-82A1-F7E74315375E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{E98AA5F9-0823-7943-9399-ED139D3CE579}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="16200" windowHeight="9970" xr2:uid="{E98AA5F9-0823-7943-9399-ED139D3CE579}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7745B56C-8897-E44A-90B6-7C6135598583}">
-  <dimension ref="A1:AF34"/>
+  <dimension ref="A1:AF32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3786,11 +3786,6 @@
         <v>226</v>
       </c>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H34">
-        <v>-1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>